<commit_message>
add unknown value test cases
</commit_message>
<xml_diff>
--- a/src/tests/integration-extra.test-cases.xlsx
+++ b/src/tests/integration-extra.test-cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayuki/WebstormProjects/JibungotoPlanet-backend/src/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11AF19B-BB6F-9F4E-9F29-934C8C189E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E7D05-3622-8A46-A93D-C5502521583F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26300" yWindow="-28300" windowWidth="22920" windowHeight="28300" activeTab="3" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="87000" yWindow="740" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="44" r:id="rId1"/>
@@ -6418,8 +6418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2C24BB-E9D1-064C-B4AA-513F56EAF28E}">
   <dimension ref="A1:M130"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -6571,8 +6571,8 @@
       <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="9" t="b">
-        <v>1</v>
+      <c r="G4" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>65</v>
@@ -11438,7 +11438,7 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -11590,8 +11590,8 @@
       <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="9" t="b">
-        <v>1</v>
+      <c r="G4" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>65</v>
@@ -16456,8 +16456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB619E8-8159-524F-8229-B401409F0BA2}">
   <dimension ref="A1:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -16609,8 +16609,8 @@
       <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="9" t="b">
-        <v>1</v>
+      <c r="G4" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>65</v>

</xml_diff>